<commit_message>
Adicionando arquivos e organizando pastas
</commit_message>
<xml_diff>
--- a/Data/DicionarioDados - Mainteer.xlsx
+++ b/Data/DicionarioDados - Mainteer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\BD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Pi2\pi-segundo-semestre-2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Cliente" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,18 @@
     <sheet name="Ordem Serviço Detalhes" sheetId="9" r:id="rId9"/>
     <sheet name="Peças_Serviço" sheetId="10" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Agendamento de Serviço'!$A$1:$E$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Cliente!$A$1:$E$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Cor!$A$1:$E$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Funcionário!$A$1:$E$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Marca!$A$1:$E$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Modelo!$A$1:$E$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Moto!$A$1:$E$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'Ordem de Serviço'!$A$1:$E$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'Ordem Serviço Detalhes'!$A$1:$E$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">Peças_Serviço!$A$1:$E$13</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="169">
   <si>
     <t>Tabela</t>
   </si>
@@ -534,6 +546,12 @@
   </si>
   <si>
     <t>ORDEM_DETALHE_ORDEM</t>
+  </si>
+  <si>
+    <t>FUN_CARGO</t>
+  </si>
+  <si>
+    <t>Cargo do Funcionário</t>
   </si>
 </sst>
 </file>
@@ -793,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -860,6 +878,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1189,9 +1216,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1207,41 +1237,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1459,17 +1489,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1477,6 +1510,7 @@
     <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
     <col min="5" max="5" width="56.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1484,41 +1518,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1662,8 +1696,8 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.39370078740157483"/>
+  <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1672,7 +1706,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1687,43 +1721,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1878,10 +1912,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1896,41 +1933,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1986,16 +2023,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2010,41 +2051,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2100,16 +2141,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2124,43 +2169,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2231,16 +2276,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2255,43 +2304,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2407,16 +2456,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2431,41 +2484,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2595,20 +2648,37 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="24">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D14" s="5">
         <v>255</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2619,16 +2689,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2643,43 +2717,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2838,16 +2912,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2862,43 +2940,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2999,6 +3077,7 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mais alguns protótipos adicionados
</commit_message>
<xml_diff>
--- a/Data/DicionarioDados - Mainteer.xlsx
+++ b/Data/DicionarioDados - Mainteer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\BD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Pi2\pi-segundo-semestre-2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Cliente" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,18 @@
     <sheet name="Ordem Serviço Detalhes" sheetId="9" r:id="rId9"/>
     <sheet name="Peças_Serviço" sheetId="10" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Agendamento de Serviço'!$A$1:$E$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Cliente!$A$1:$E$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Cor!$A$1:$E$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Funcionário!$A$1:$E$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Marca!$A$1:$E$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Modelo!$A$1:$E$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Moto!$A$1:$E$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'Ordem de Serviço'!$A$1:$E$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'Ordem Serviço Detalhes'!$A$1:$E$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">Peças_Serviço!$A$1:$E$13</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="169">
   <si>
     <t>Tabela</t>
   </si>
@@ -534,6 +546,12 @@
   </si>
   <si>
     <t>ORDEM_DETALHE_ORDEM</t>
+  </si>
+  <si>
+    <t>FUN_CARGO</t>
+  </si>
+  <si>
+    <t>Cargo do Funcionário</t>
   </si>
 </sst>
 </file>
@@ -793,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -860,6 +878,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1189,9 +1216,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1207,41 +1237,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1459,17 +1489,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1477,6 +1510,7 @@
     <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
     <col min="5" max="5" width="56.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1484,41 +1518,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1662,8 +1696,8 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.39370078740157483"/>
+  <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1672,7 +1706,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1687,43 +1721,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1878,10 +1912,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1896,41 +1933,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1986,16 +2023,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2010,41 +2051,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2100,16 +2141,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2124,43 +2169,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2231,16 +2276,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2255,43 +2304,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2407,16 +2456,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="56" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2431,41 +2484,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2595,20 +2648,37 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="24">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D14" s="5">
         <v>255</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2619,16 +2689,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2643,43 +2717,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2838,16 +2912,20 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2862,43 +2940,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2999,6 +3077,7 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizando o Dicionário de Dados
</commit_message>
<xml_diff>
--- a/Data/DicionarioDados - Mainteer.xlsx
+++ b/Data/DicionarioDados - Mainteer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Pi2\pi-segundo-semestre-2025\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Pi2\pi-segundo-semestre-2025\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Cliente" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Peças_Serviço" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'Agendamento de Serviço'!$A$1:$E$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Agendamento de Serviço'!$A$1:$E$12</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Cliente!$A$1:$E$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Cor!$A$1:$E$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">Funcionário!$A$1:$E$14</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="176">
   <si>
     <t>Tabela</t>
   </si>
@@ -161,9 +161,6 @@
     <t>MODELO_MARCA</t>
   </si>
   <si>
-    <t>Possui FK do Funcionário e Moto</t>
-  </si>
-  <si>
     <t>AGEN_ID</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Armazenará informações dos agendamentos de Serviço</t>
   </si>
   <si>
-    <t>Possui FK Funcionario e Moto</t>
-  </si>
-  <si>
     <t>Armazenará os dados dos Funcionários</t>
   </si>
   <si>
@@ -552,6 +546,33 @@
   </si>
   <si>
     <t>Cargo do Funcionário</t>
+  </si>
+  <si>
+    <t>Possui FK Funcionario, Moto e Cliente</t>
+  </si>
+  <si>
+    <t>ORDEM_CLIENTE</t>
+  </si>
+  <si>
+    <t>NOT NULL, DEFAULT TIMESTAMP</t>
+  </si>
+  <si>
+    <t>NOT NULL, DEFAULT 'A'</t>
+  </si>
+  <si>
+    <t>AGEN_HORA</t>
+  </si>
+  <si>
+    <t>Hora do Agendamento</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>AGEN_CLIENTE</t>
+  </si>
+  <si>
+    <t>Possui FK do Funcionário, Moto e Cliente</t>
   </si>
 </sst>
 </file>
@@ -811,7 +832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -889,6 +910,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -935,6 +968,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1237,41 +1273,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1287,7 +1323,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1295,14 +1331,14 @@
         <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1310,16 +1346,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="9">
         <v>100</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1327,10 +1363,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="9">
         <v>10</v>
@@ -1342,10 +1378,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="9">
         <v>20</v>
@@ -1357,16 +1393,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="9">
         <v>50</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1374,10 +1410,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" s="9">
         <v>20</v>
@@ -1389,16 +1425,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" s="9">
         <v>15</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1406,16 +1442,16 @@
         <v>15</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D13" s="9">
         <v>15</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1423,16 +1459,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D14" s="9">
         <v>100</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1440,14 +1476,14 @@
         <v>17</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1455,10 +1491,10 @@
         <v>18</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D16" s="9">
         <v>250</v>
@@ -1470,16 +1506,16 @@
         <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D17" s="5">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1501,8 +1537,8 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1518,41 +1554,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1568,67 +1604,67 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D7" s="9">
         <v>1</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="9">
         <v>50</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="9">
         <v>100</v>
@@ -1637,54 +1673,54 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
@@ -1721,43 +1757,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1773,7 +1809,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1781,14 +1817,14 @@
         <v>22</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1796,10 +1832,10 @@
         <v>23</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
@@ -1809,16 +1845,16 @@
         <v>24</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="9">
         <v>10</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1826,10 +1862,10 @@
         <v>25</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="9">
         <v>250</v>
@@ -1841,16 +1877,16 @@
         <v>26</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1858,14 +1894,14 @@
         <v>27</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1873,14 +1909,14 @@
         <v>28</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1888,14 +1924,14 @@
         <v>29</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1933,41 +1969,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -1983,7 +2019,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1991,14 +2027,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2006,10 +2042,10 @@
         <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3">
         <v>50</v>
@@ -2051,41 +2087,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2101,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2109,14 +2145,14 @@
         <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2124,10 +2160,10 @@
         <v>33</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3">
         <v>50</v>
@@ -2169,43 +2205,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
+      <c r="B2" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2221,7 +2257,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2229,14 +2265,14 @@
         <v>35</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2244,10 +2280,10 @@
         <v>36</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="9">
         <v>50</v>
@@ -2259,14 +2295,14 @@
         <v>37</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2286,10 +2322,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2304,43 +2340,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2356,97 +2392,125 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
-        <v>92</v>
+      <c r="C6" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29" t="s">
         <v>93</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="9">
-        <v>250</v>
-      </c>
-      <c r="E8" s="10"/>
+        <v>171</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="28">
+        <v>250</v>
+      </c>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="B11" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6" t="s">
-        <v>75</v>
+      <c r="B12" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2469,7 +2533,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2484,41 +2548,41 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2534,67 +2598,67 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="9">
         <v>100</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="9">
         <v>15</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="9">
         <v>15</v>
@@ -2603,83 +2667,83 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D11" s="9">
         <v>1</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" s="9">
         <v>100</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D13" s="24">
         <v>1</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D14" s="5">
         <v>255</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2699,10 +2763,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2717,43 +2781,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
+      <c r="B2" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
+      <c r="B3" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2769,140 +2833,155 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
-        <v>92</v>
+      <c r="C6" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10" t="s">
-        <v>95</v>
+        <v>56</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="9">
+        <v>58</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="28">
         <v>100</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10" t="s">
-        <v>95</v>
+        <v>59</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10" t="s">
-        <v>95</v>
+        <v>60</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="9">
+        <v>61</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="28">
         <v>250</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="13" t="s">
+      <c r="C13" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6" t="s">
-        <v>95</v>
+      <c r="C14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="46"/>
+      <c r="E15" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2940,43 +3019,43 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -2992,82 +3071,82 @@
         <v>5</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>